<commit_message>
Feat : [#2} 텍스트1 추가
메인씬에서 게임씬으로 넘어가지 않는 문제 있음
</commit_message>
<xml_diff>
--- a/SDL Game Framework/SDL Game Framework/test.xlsx
+++ b/SDL Game Framework/SDL Game Framework/test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AA7528-420C-4BF3-A0A5-3B2E76D436D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,14 +30,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>테스트입니다.</t>
+    <t>메롱입니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,14 +355,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>